<commit_message>
New Data missing and xml changes
</commit_message>
<xml_diff>
--- a/src/test/java/Orders/Data/Orders.xlsx
+++ b/src/test/java/Orders/Data/Orders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APIAutomation\Automation_OMSAPI\src\test\java\Orders\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F8D578-9724-4555-B6DB-F74D328AFFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDA3895-1716-4EB6-A625-E64C5DAC142B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="357" activeTab="1" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="357" firstSheet="2" activeTab="4" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
   </bookViews>
   <sheets>
     <sheet name="OrderSubscriptions" sheetId="14" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="450">
   <si>
     <t>Content_Type</t>
   </si>
@@ -2481,6 +2481,9 @@
     "Text":"TestCase_VTRAD-C990-B"
  }</t>
   </si>
+  <si>
+    <t>20.0</t>
+  </si>
 </sst>
 </file>
 
@@ -2489,7 +2492,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2543,6 +2546,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2579,7 +2596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -2625,6 +2642,22 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2942,8 +2975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA8D027-6E8C-4E62-B2F3-94FA83F4F6D0}">
   <dimension ref="A1:AK27"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AE30" sqref="AE30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4910,229 +4943,229 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+    <row r="18" spans="1:37" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="17" t="s">
+      <c r="D18" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="F18" s="18">
-        <v>200</v>
-      </c>
-      <c r="G18" s="17" t="s">
+      <c r="F18" s="24">
+        <v>200</v>
+      </c>
+      <c r="G18" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="17">
-        <v>200</v>
-      </c>
-      <c r="J18" s="17" t="s">
+      <c r="I18" s="23">
+        <v>200</v>
+      </c>
+      <c r="J18" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="25">
         <v>3</v>
       </c>
-      <c r="L18" s="17">
-        <v>1</v>
-      </c>
-      <c r="M18" s="17" t="s">
+      <c r="L18" s="23">
+        <v>1</v>
+      </c>
+      <c r="M18" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="N18" s="17" t="s">
+      <c r="N18" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="O18" s="11" t="s">
+      <c r="O18" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="P18" s="17" t="s">
+      <c r="P18" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="Q18" s="20">
+      <c r="Q18" s="27">
         <v>0</v>
       </c>
-      <c r="R18" s="20">
+      <c r="R18" s="27">
         <v>222</v>
       </c>
-      <c r="S18" s="17">
+      <c r="S18" s="23" t="s">
+        <v>449</v>
+      </c>
+      <c r="T18" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="U18" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="V18" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="W18" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="X18" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y18" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z18" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA18" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB18" s="27">
         <v>0</v>
       </c>
-      <c r="T18" s="17" t="s">
+      <c r="AC18" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD18" s="27">
+        <v>222</v>
+      </c>
+      <c r="AE18" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="U18" s="17" t="s">
+      <c r="AF18" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG18" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH18" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI18" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ18" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK18" s="22" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="F19" s="24">
+        <v>200</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="23">
+        <v>200</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="25">
+        <v>3</v>
+      </c>
+      <c r="L19" s="23">
+        <v>1</v>
+      </c>
+      <c r="M19" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="N19" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="P19" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q19" s="27">
+        <v>0</v>
+      </c>
+      <c r="R19" s="27">
+        <v>222</v>
+      </c>
+      <c r="S19" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="T19" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="U19" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="V18" s="17" t="s">
+      <c r="V19" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="W18" s="17" t="s">
+      <c r="W19" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="X18" s="17" t="s">
+      <c r="X19" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="Y18" s="17" t="s">
+      <c r="Y19" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="Z18" s="17" t="s">
+      <c r="Z19" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="AA18" s="17" t="s">
+      <c r="AA19" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="AB18" s="20">
+      <c r="AB19" s="27">
         <v>0</v>
       </c>
-      <c r="AC18" s="17" t="s">
+      <c r="AC19" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="AD18" s="20">
+      <c r="AD19" s="27">
         <v>222</v>
       </c>
-      <c r="AE18" s="17" t="s">
+      <c r="AE19" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="AF18" s="17" t="s">
+      <c r="AF19" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="AG18" s="17" t="s">
+      <c r="AG19" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AH18" s="17" t="s">
+      <c r="AH19" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="AI18" s="17" t="s">
+      <c r="AI19" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="AJ18" s="17" t="s">
+      <c r="AJ19" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="AK18" s="16" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>269</v>
-      </c>
-      <c r="F19" s="18">
-        <v>200</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="17">
-        <v>200</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19" s="19">
-        <v>3</v>
-      </c>
-      <c r="L19" s="17">
-        <v>1</v>
-      </c>
-      <c r="M19" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="N19" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="O19" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="P19" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q19" s="20">
-        <v>0</v>
-      </c>
-      <c r="R19" s="20">
-        <v>222</v>
-      </c>
-      <c r="S19" s="17">
-        <v>0</v>
-      </c>
-      <c r="T19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="U19" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="V19" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="W19" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="X19" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y19" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z19" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA19" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB19" s="20">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD19" s="20">
-        <v>222</v>
-      </c>
-      <c r="AE19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG19" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH19" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI19" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ19" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK19" s="16" t="s">
+      <c r="AK19" s="22" t="s">
         <v>284</v>
       </c>
     </row>
@@ -5249,116 +5282,116 @@
         <v>285</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:37" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="17" t="s">
+      <c r="D21" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="23" t="s">
         <v>267</v>
       </c>
-      <c r="F21" s="18">
-        <v>200</v>
-      </c>
-      <c r="G21" s="17" t="s">
+      <c r="F21" s="24">
+        <v>200</v>
+      </c>
+      <c r="G21" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="17">
-        <v>200</v>
-      </c>
-      <c r="J21" s="17" t="s">
+      <c r="I21" s="23">
+        <v>200</v>
+      </c>
+      <c r="J21" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K21" s="19">
+      <c r="K21" s="25">
         <v>3</v>
       </c>
-      <c r="L21" s="17">
-        <v>1</v>
-      </c>
-      <c r="M21" s="17" t="s">
+      <c r="L21" s="23">
+        <v>1</v>
+      </c>
+      <c r="M21" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="N21" s="17" t="s">
+      <c r="N21" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="11" t="s">
+      <c r="O21" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="P21" s="17" t="s">
+      <c r="P21" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="Q21" s="20">
+      <c r="Q21" s="27">
         <v>0</v>
       </c>
-      <c r="R21" s="20">
+      <c r="R21" s="27">
         <v>222</v>
       </c>
-      <c r="S21" s="17">
+      <c r="S21" s="23" t="s">
+        <v>449</v>
+      </c>
+      <c r="T21" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="U21" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="V21" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="W21" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="X21" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y21" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z21" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA21" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB21" s="27">
         <v>0</v>
       </c>
-      <c r="T21" s="17" t="s">
+      <c r="AC21" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD21" s="27">
+        <v>222</v>
+      </c>
+      <c r="AE21" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="U21" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="V21" s="17" t="s">
+      <c r="AF21" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG21" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH21" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="W21" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="X21" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y21" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z21" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA21" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB21" s="20">
-        <v>0</v>
-      </c>
-      <c r="AC21" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD21" s="20">
-        <v>222</v>
-      </c>
-      <c r="AE21" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF21" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG21" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH21" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI21" s="17" t="s">
+      <c r="AI21" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="AJ21" s="17" t="s">
+      <c r="AJ21" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="AK21" s="16" t="s">
+      <c r="AK21" s="22" t="s">
         <v>286</v>
       </c>
     </row>
@@ -5927,116 +5960,116 @@
         <v>291</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+    <row r="27" spans="1:37" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="17" t="s">
+      <c r="D27" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="23" t="s">
         <v>280</v>
       </c>
-      <c r="F27" s="18">
-        <v>200</v>
-      </c>
-      <c r="G27" s="17" t="s">
+      <c r="F27" s="24">
+        <v>200</v>
+      </c>
+      <c r="G27" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="17" t="s">
+      <c r="H27" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I27" s="17">
-        <v>200</v>
-      </c>
-      <c r="J27" s="17" t="s">
+      <c r="I27" s="23">
+        <v>200</v>
+      </c>
+      <c r="J27" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K27" s="19">
+      <c r="K27" s="25">
         <v>3</v>
       </c>
-      <c r="L27" s="17">
-        <v>1</v>
-      </c>
-      <c r="M27" s="17" t="s">
+      <c r="L27" s="23">
+        <v>1</v>
+      </c>
+      <c r="M27" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="N27" s="17" t="s">
+      <c r="N27" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="O27" s="11" t="s">
+      <c r="O27" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="P27" s="17" t="s">
+      <c r="P27" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="Q27" s="20">
+      <c r="Q27" s="27">
         <v>0</v>
       </c>
-      <c r="R27" s="20">
+      <c r="R27" s="27">
         <v>222</v>
       </c>
-      <c r="S27" s="17">
+      <c r="S27" s="23" t="s">
+        <v>320</v>
+      </c>
+      <c r="T27" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="U27" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="V27" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="W27" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="X27" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y27" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z27" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA27" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB27" s="27">
         <v>0</v>
       </c>
-      <c r="T27" s="17" t="s">
+      <c r="AC27" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD27" s="27">
+        <v>222</v>
+      </c>
+      <c r="AE27" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="U27" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="V27" s="17" t="s">
+      <c r="AF27" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG27" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH27" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="W27" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="X27" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y27" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z27" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA27" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB27" s="20">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD27" s="20">
-        <v>222</v>
-      </c>
-      <c r="AE27" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF27" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG27" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH27" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI27" s="17" t="s">
+      <c r="AI27" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="AJ27" s="17" t="s">
+      <c r="AJ27" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="AK27" s="16" t="s">
+      <c r="AK27" s="22" t="s">
         <v>292</v>
       </c>
     </row>
@@ -6051,7 +6084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{743E006D-5A16-4AF8-97F0-E530401F0C8B}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -8111,8 +8144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC32307C-E7E7-45A6-BDDF-2098EC346FB1}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E7:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8290,7 +8323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>422</v>
       </c>
@@ -8303,7 +8336,7 @@
       <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="21" t="s">
         <v>421</v>
       </c>
       <c r="F4">

</xml_diff>